<commit_message>
Database addition implemented, seems to be a LOT slower than generator -> set -> db
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Exponential Growth.xlsx
+++ b/Dissertation/Research/Exponential Growth.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
   </bookViews>
   <sheets>
     <sheet name="G3 - None" sheetId="1" r:id="rId1"/>
@@ -2847,6 +2847,12 @@
                 <c:pt idx="7">
                   <c:v>839157</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>4540668</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24563253</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3356,6 +3362,12 @@
                 <c:pt idx="7">
                   <c:v>81.674999999999997</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>457.68599999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2411</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3465,34 +3477,34 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>5.0649214436777352E-3</c:v>
+                  <c:v>5.1473333725508795E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0259685774710941E-2</c:v>
+                  <c:v>2.0589333490203518E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.116858598619923E-2</c:v>
+                  <c:v>9.2652000705915824E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46597277281835164</c:v>
+                  <c:v>0.4735546702746809</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5932397791630004</c:v>
+                  <c:v>2.6354346867460503</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.467626118739098</c:v>
+                  <c:v>13.686759437612787</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.173564067064959</c:v>
+                  <c:v>76.396721915400164</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>413.67745891237905</c:v>
+                  <c:v>420.40845320309307</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2355.8624219493217</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>12410.220761220171</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3618,46 +3630,46 @@
                   <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0649214436777352E-3</c:v>
+                  <c:v>5.1473333725508795E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5653429230626554E-2</c:v>
+                  <c:v>2.6495040848176013E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12993260381406965</c:v>
+                  <c:v>0.13637880796491517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.65809843129076495</c:v>
+                  <c:v>0.70198718954651551</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.333216856695274</c:v>
+                  <c:v>3.6133620878559793</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.882481533903992</c:v>
+                  <c:v>18.599179261931205</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>85.50844274356372</c:v>
+                  <c:v>95.736176116994727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>433.09354526736576</c:v>
+                  <c:v>492.78601428741547</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2193.5847845430949</c:v>
+                  <c:v>2536.5338968679484</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11110.334613757526</c:v>
+                  <c:v>13056.385577954923</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>56272.972031655489</c:v>
+                  <c:v>67205.569210299378</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>285018.18274260935</c:v>
+                  <c:v>345929.46921745187</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1443594.7056111016</c:v>
+                  <c:v>1780614.3014518023</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7311693.7804293158</c:v>
+                  <c:v>9165415.4175042342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8007,7 +8019,7 @@
   <dimension ref="B2:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G22"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8409,7 +8421,7 @@
         <v>0.10024077943288258</v>
       </c>
       <c r="I14" s="11">
-        <f t="shared" si="0"/>
+        <f>6^B14</f>
         <v>60466176</v>
       </c>
       <c r="J14" s="3">
@@ -8700,8 +8712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113CE139-0867-4B85-B215-793B955C4FB4}">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9325,8 +9337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74A1760-7553-4645-8968-6CCC96E3951B}">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9349,14 +9361,14 @@
       </c>
       <c r="D2" s="3">
         <f>AVERAGE(D6:D20)</f>
-        <v>5.0649214436777354</v>
+        <v>5.1473333725508796</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="3">
         <f>AVERAGE(J6:J20)</f>
-        <v>3.8257646742988926E-5</v>
+        <v>4.9069743037269158E-5</v>
       </c>
     </row>
     <row r="4" spans="2:10" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -9424,19 +9436,19 @@
       </c>
       <c r="E6" s="9">
         <f>C5*$D$2</f>
-        <v>5.0649214436777352E-3</v>
+        <v>5.1473333725508795E-3</v>
       </c>
       <c r="F6" s="10">
         <f>IF(C6&lt;&gt;0,((ABS(E6-C6))/C6),"")</f>
-        <v>0.26623036091943375</v>
+        <v>0.28683334313771985</v>
       </c>
       <c r="G6" s="9">
         <f>G5*$D$2</f>
-        <v>5.0649214436777352E-3</v>
+        <v>5.1473333725508795E-3</v>
       </c>
       <c r="H6" s="10">
         <f>IF(C6&lt;&gt;0,((ABS(G6-C6))/C6),"")</f>
-        <v>0.26623036091943375</v>
+        <v>0.28683334313771985</v>
       </c>
       <c r="I6" s="11">
         <v>33</v>
@@ -9459,19 +9471,19 @@
       </c>
       <c r="E7" s="9">
         <f t="shared" ref="E7:E20" si="1">C6*$D$2</f>
-        <v>2.0259685774710941E-2</v>
+        <v>2.0589333490203518E-2</v>
       </c>
       <c r="F7" s="10">
         <f t="shared" ref="F7:F20" si="2">IF(C7&lt;&gt;0,((ABS(E7-C7))/C7),"")</f>
-        <v>0.12553809859505236</v>
+        <v>0.14385186056686219</v>
       </c>
       <c r="G7" s="9">
         <f>G6*$D$2</f>
-        <v>2.5653429230626554E-2</v>
+        <v>2.6495040848176013E-2</v>
       </c>
       <c r="H7" s="10">
         <f t="shared" ref="H7:H20" si="3">IF(C7&lt;&gt;0,((ABS(G7-C7))/C7),"")</f>
-        <v>0.42519051281258646</v>
+        <v>0.47194671378755637</v>
       </c>
       <c r="I7" s="11">
         <v>180</v>
@@ -9494,19 +9506,19 @@
       </c>
       <c r="E8" s="9">
         <f t="shared" si="1"/>
-        <v>9.116858598619923E-2</v>
+        <v>9.2652000705915824E-2</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="2"/>
-        <v>9.037108845660528E-3</v>
+        <v>7.0869641947372344E-3</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" ref="G8:G20" si="4">G7*$D$2</f>
-        <v>0.12993260381406965</v>
+        <v>0.13637880796491517</v>
       </c>
       <c r="H8" s="10">
         <f t="shared" si="3"/>
-        <v>0.41231091102249623</v>
+        <v>0.48237834744473007</v>
       </c>
       <c r="I8" s="11">
         <v>976</v>
@@ -9529,19 +9541,19 @@
       </c>
       <c r="E9" s="9">
         <f t="shared" si="1"/>
-        <v>0.46597277281835164</v>
+        <v>0.4735546702746809</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="2"/>
-        <v>8.9896928089156961E-2</v>
+        <v>7.5088534619763891E-2</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" si="4"/>
-        <v>0.65809843129076495</v>
+        <v>0.70198718954651551</v>
       </c>
       <c r="H9" s="10">
         <f t="shared" si="3"/>
-        <v>0.28534849861477529</v>
+        <v>0.3710687295830381</v>
       </c>
       <c r="I9" s="11">
         <v>5286</v>
@@ -9564,19 +9576,19 @@
       </c>
       <c r="E10" s="9">
         <f t="shared" si="1"/>
-        <v>2.5932397791630004</v>
+        <v>2.6354346867460503</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="2"/>
-        <v>2.4731184970665437E-2</v>
+        <v>8.8624720774537445E-3</v>
       </c>
       <c r="G10" s="9">
         <f t="shared" si="4"/>
-        <v>3.333216856695274</v>
+        <v>3.6133620878559793</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="3"/>
-        <v>0.25356030714376615</v>
+        <v>0.35891767125083851</v>
       </c>
       <c r="I10" s="11">
         <v>28635</v>
@@ -9599,19 +9611,19 @@
       </c>
       <c r="E11" s="9">
         <f t="shared" si="1"/>
-        <v>13.467626118739098</v>
+        <v>13.686759437612787</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" si="2"/>
-        <v>9.2600315406340297E-2</v>
+        <v>7.7835909067997117E-2</v>
       </c>
       <c r="G11" s="9">
         <f t="shared" si="4"/>
-        <v>16.882481533903992</v>
+        <v>18.599179261931205</v>
       </c>
       <c r="H11" s="10">
         <f t="shared" si="3"/>
-        <v>0.13748022732138465</v>
+        <v>0.25314507896046384</v>
       </c>
       <c r="I11" s="11">
         <v>155040</v>
@@ -9634,19 +9646,19 @@
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>75.173564067064959</v>
+        <v>76.396721915400164</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="2"/>
-        <v>7.9601297005632551E-2</v>
+        <v>6.4625382119373534E-2</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" si="4"/>
-        <v>85.50844274356372</v>
+        <v>95.736176116994727</v>
       </c>
       <c r="H12" s="10">
         <f t="shared" si="3"/>
-        <v>4.6935325908340646E-2</v>
+        <v>0.17216009938163124</v>
       </c>
       <c r="I12" s="11">
         <v>839157</v>
@@ -9660,62 +9672,70 @@
       <c r="B13" s="8">
         <v>9</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="str">
+      <c r="C13" s="9">
+        <v>457.68599999999998</v>
+      </c>
+      <c r="D13" s="9">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5.6037465564738289</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>413.67745891237905</v>
-      </c>
-      <c r="F13" s="10" t="str">
+        <v>420.40845320309307</v>
+      </c>
+      <c r="F13" s="10">
         <f t="shared" si="2"/>
-        <v/>
+        <v>8.1447863375560772E-2</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" si="4"/>
-        <v>433.09354526736576</v>
-      </c>
-      <c r="H13" s="10" t="str">
+        <v>492.78601428741547</v>
+      </c>
+      <c r="H13" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I13" s="11"/>
+        <v>7.669016375291246E-2</v>
+      </c>
+      <c r="I13" s="11">
+        <v>4540668</v>
+      </c>
       <c r="J13" s="12">
         <f>C13/SUM(I$5:I13)</f>
-        <v>0</v>
+        <v>8.2170118713151798E-5</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
         <v>10</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="str">
+      <c r="C14" s="9">
+        <v>2411</v>
+      </c>
+      <c r="D14" s="9">
         <f>IF(C13&lt;&gt;0,IF(C14&lt;&gt;0,C14/C13,""),"")</f>
-        <v/>
+        <v>5.2678036907399397</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="10" t="str">
+        <v>2355.8624219493217</v>
+      </c>
+      <c r="F14" s="10">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2.2869173807830052E-2</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="4"/>
-        <v>2193.5847845430949</v>
-      </c>
-      <c r="H14" s="10" t="str">
+        <v>2536.5338968679484</v>
+      </c>
+      <c r="H14" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I14" s="11"/>
+        <v>5.2067149260866218E-2</v>
+      </c>
+      <c r="I14" s="11">
+        <v>24563253</v>
+      </c>
       <c r="J14" s="12">
         <f>C14/SUM(I$5:I14)</f>
-        <v>0</v>
+        <v>8.0011325701051541E-5</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -9729,7 +9749,7 @@
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12410.220761220171</v>
       </c>
       <c r="F15" s="10" t="str">
         <f t="shared" si="2"/>
@@ -9737,7 +9757,7 @@
       </c>
       <c r="G15" s="9">
         <f t="shared" si="4"/>
-        <v>11110.334613757526</v>
+        <v>13056.385577954923</v>
       </c>
       <c r="H15" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9768,7 +9788,7 @@
       </c>
       <c r="G16" s="9">
         <f t="shared" si="4"/>
-        <v>56272.972031655489</v>
+        <v>67205.569210299378</v>
       </c>
       <c r="H16" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9799,7 +9819,7 @@
       </c>
       <c r="G17" s="9">
         <f t="shared" si="4"/>
-        <v>285018.18274260935</v>
+        <v>345929.46921745187</v>
       </c>
       <c r="H17" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9830,7 +9850,7 @@
       </c>
       <c r="G18" s="9">
         <f t="shared" si="4"/>
-        <v>1443594.7056111016</v>
+        <v>1780614.3014518023</v>
       </c>
       <c r="H18" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9861,7 +9881,7 @@
       </c>
       <c r="G19" s="9">
         <f t="shared" si="4"/>
-        <v>7311693.7804293158</v>
+        <v>9165415.4175042342</v>
       </c>
       <c r="H19" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9892,7 +9912,7 @@
       </c>
       <c r="G20" s="9">
         <f t="shared" si="4"/>
-        <v>37033154.618101567</v>
+        <v>47177448.651811898</v>
       </c>
       <c r="H20" s="10" t="str">
         <f t="shared" si="3"/>
@@ -9908,7 +9928,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J6:J11" formulaRange="1"/>
+    <ignoredError sqref="J6:J13" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Thistlethwaite-esque method all but complete, need to change DB structure to hold serialized lists and not strings though
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Exponential Growth.xlsx
+++ b/Dissertation/Research/Exponential Growth.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Will Garside\Documents\Projects\Active\RubiksSolver\Dissertation\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Will Garside\Documents\Projects\Active\CubeSolver\Dissertation\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="3" activeTab="3" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
   </bookViews>
   <sheets>
     <sheet name="G3 - None" sheetId="1" r:id="rId1"/>
     <sheet name="G3 - Dup Check" sheetId="2" r:id="rId2"/>
     <sheet name="G0 - Dup Check" sheetId="4" r:id="rId3"/>
+    <sheet name="Phase 4 Generation" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171026"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
   <si>
     <t>Depth</t>
   </si>
@@ -60,6 +61,18 @@
   <si>
     <t>Average Time per Position:</t>
   </si>
+  <si>
+    <t>Growth Factor Growth Factor</t>
+  </si>
+  <si>
+    <t>Predicted Growth</t>
+  </si>
+  <si>
+    <t>Predicted Growth Factor</t>
+  </si>
+  <si>
+    <t>Pos Count</t>
+  </si>
 </sst>
 </file>
 
@@ -69,8 +82,16 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -137,6 +158,18 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8712,8 +8745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113CE139-0867-4B85-B215-793B955C4FB4}">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9338,7 +9371,7 @@
   <dimension ref="B2:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9932,4 +9965,1033 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C26503-4535-4175-8A49-8C86F5FB11B3}">
+  <dimension ref="B2:S19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="4" customWidth="1"/>
+    <col min="12" max="15" width="9.140625" style="3"/>
+    <col min="16" max="16" width="14.85546875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="12" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(E6:E19)</f>
+        <v>3.1059535652336456</v>
+      </c>
+      <c r="F2" s="3">
+        <f>AVERAGE(F6:F19)</f>
+        <v>0.87605519977150292</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6</v>
+      </c>
+      <c r="D5" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="str">
+        <f t="shared" ref="F5:F15" si="0">IF(E4&lt;&gt;0,IF(E5&lt;&gt;"",E5/E4,""),"")</f>
+        <v/>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="4">
+        <f>D5</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="15">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9" t="str">
+        <f t="shared" ref="P5:P19" si="1">IF(O4&lt;&gt;0,IF(O5&lt;&gt;"",O5/O4,""),"")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="8"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>27</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" ref="E6:E13" si="2">IF(D5&lt;&gt;0,IF(D6&lt;&gt;0,D6/D5,""),"")</f>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="F6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="10">
+        <f>IF(D6&lt;&gt;0,((ABS(H6-D6))/D6),"")</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="9">
+        <f>E6</f>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="K6" s="4">
+        <f>J6*K5</f>
+        <v>2.5999999999999995E-2</v>
+      </c>
+      <c r="M6" s="8">
+        <v>2</v>
+      </c>
+      <c r="N6" s="15">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="O6" s="9">
+        <f t="shared" ref="O6:O13" si="3">IF(N5&lt;&gt;0,IF(N6&lt;&gt;0,N6/N5,""),"")</f>
+        <v>1.2325581395348837</v>
+      </c>
+      <c r="P6" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="10">
+        <f>IF(N6&lt;&gt;0,((ABS(R6-N6))/N6),"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>120</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="2"/>
+        <v>5.0384615384615392</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.96893491124260378</v>
+      </c>
+      <c r="G7" s="9">
+        <f>IF(E6&lt;&gt;"",$F$2*E6,"")</f>
+        <v>4.5554870388118145</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" ref="H7:H19" si="4">IF(D6&lt;&gt;0, D6*G7,"")</f>
+        <v>0.11844266300910718</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" ref="I7:I19" si="5">IF(D7&lt;&gt;0,((ABS(H7-D7))/D7),"")</f>
+        <v>9.5857534281624635E-2</v>
+      </c>
+      <c r="J7" s="9">
+        <f>J6*$F$2</f>
+        <v>4.5554870388118145</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" ref="K7:K19" si="6">J7*K6</f>
+        <v>0.11844266300910715</v>
+      </c>
+      <c r="M7" s="8">
+        <v>3</v>
+      </c>
+      <c r="N7" s="15">
+        <v>2.7E-2</v>
+      </c>
+      <c r="O7" s="9">
+        <f t="shared" si="3"/>
+        <v>0.50943396226415094</v>
+      </c>
+      <c r="P7" s="9">
+        <f t="shared" si="1"/>
+        <v>0.41331434674261303</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" ref="Q7:Q19" si="7">IF(O6&lt;&gt;"",$F$2*O6,"")</f>
+        <v>1.0797889671602245</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" ref="R7:R19" si="8">IF(N6&lt;&gt;0, N6*Q7,"")</f>
+        <v>5.7228815259491903E-2</v>
+      </c>
+      <c r="S7" s="10">
+        <f t="shared" ref="S7:S19" si="9">IF(N7&lt;&gt;0,((ABS(R7-N7))/N7),"")</f>
+        <v>1.1195857503515521</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>519</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="2"/>
+        <v>4.7251908396946565</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9378241361226034</v>
+      </c>
+      <c r="G8" s="9">
+        <f>IF(E7&lt;&gt;"",$F$2*E7,"")</f>
+        <v>4.413970429617958</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="4"/>
+        <v>0.57823012627995252</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="5"/>
+        <v>6.5864093247249567E-2</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" ref="J8:J19" si="10">J7*$F$2</f>
+        <v>3.9908581078427763</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="6"/>
+        <v>0.47268786198438495</v>
+      </c>
+      <c r="M8" s="8">
+        <v>4</v>
+      </c>
+      <c r="N8" s="15">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="O8" s="9">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="P8" s="9">
+        <f t="shared" si="1"/>
+        <v>2.617283950617284</v>
+      </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="7"/>
+        <v>0.44629227158170903</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="8"/>
+        <v>1.2049891332706144E-2</v>
+      </c>
+      <c r="S8" s="10">
+        <f t="shared" si="9"/>
+        <v>0.66528079631371817</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1932</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2.6909999999999998</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="2"/>
+        <v>4.3473344103392568</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.92003361511218518</v>
+      </c>
+      <c r="G9" s="9">
+        <f>IF(E8&lt;&gt;"",$F$2*E8,"")</f>
+        <v>4.1395280050271781</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="4"/>
+        <v>2.5623678351118233</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="5"/>
+        <v>4.7800878813889461E-2</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="10"/>
+        <v>3.4962119969259255</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="6"/>
+        <v>1.6526169738710728</v>
+      </c>
+      <c r="M9" s="8">
+        <v>5</v>
+      </c>
+      <c r="N9" s="15">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="O9" s="9">
+        <f t="shared" si="3"/>
+        <v>6.5555555555555554</v>
+      </c>
+      <c r="P9" s="9">
+        <f t="shared" si="1"/>
+        <v>4.916666666666667</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="7"/>
+        <v>1.1680735996953371</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="8"/>
+        <v>4.2050649589032131E-2</v>
+      </c>
+      <c r="S9" s="10">
+        <f t="shared" si="9"/>
+        <v>0.82181928140240623</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6484</v>
+      </c>
+      <c r="D10" s="14">
+        <v>9.5120000000000005</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5347454477889264</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.81308340103357324</v>
+      </c>
+      <c r="G10" s="9">
+        <f>IF(E9&lt;&gt;"",$F$2*E9,"")</f>
+        <v>3.8085049153232866</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="4"/>
+        <v>10.248686727134963</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="5"/>
+        <v>7.7448142045307256E-2</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="10"/>
+        <v>3.0628746994104668</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="6"/>
+        <v>5.061758717085997</v>
+      </c>
+      <c r="M10" s="8">
+        <v>6</v>
+      </c>
+      <c r="N10" s="15">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="O10" s="9">
+        <f t="shared" si="3"/>
+        <v>1.4745762711864407</v>
+      </c>
+      <c r="P10" s="9">
+        <f t="shared" si="1"/>
+        <v>0.22493536340132148</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="7"/>
+        <v>5.7430285318354075</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="8"/>
+        <v>1.3553547335131562</v>
+      </c>
+      <c r="S10" s="10">
+        <f t="shared" si="9"/>
+        <v>2.894697510095277</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8">
+        <v>20310</v>
+      </c>
+      <c r="D11" s="14">
+        <v>32.844000000000001</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="2"/>
+        <v>3.452901597981497</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9768458999335794</v>
+      </c>
+      <c r="G11" s="9">
+        <f>IF(E10&lt;&gt;"",$F$2*E10,"")</f>
+        <v>3.0966321294041386</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="4"/>
+        <v>29.455164814892168</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="5"/>
+        <v>0.10317973404907542</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="10"/>
+        <v>2.6832473066671185</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="6"/>
+        <v>13.58195044461981</v>
+      </c>
+      <c r="M11" s="8">
+        <v>7</v>
+      </c>
+      <c r="N11" s="15">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="O11" s="9">
+        <f t="shared" si="3"/>
+        <v>1.8505747126436782</v>
+      </c>
+      <c r="P11" s="9">
+        <f t="shared" si="1"/>
+        <v>1.2549874488043335</v>
+      </c>
+      <c r="Q11" s="9">
+        <f t="shared" si="7"/>
+        <v>1.2918102098325552</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" si="8"/>
+        <v>0.44954995302172918</v>
+      </c>
+      <c r="S11" s="10">
+        <f t="shared" si="9"/>
+        <v>0.30194106673644538</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8">
+        <v>55034</v>
+      </c>
+      <c r="D12" s="14">
+        <v>108.654</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="2"/>
+        <v>3.3081841432225061</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.95808816131812446</v>
+      </c>
+      <c r="G12" s="9">
+        <f>IF(E11&lt;&gt;"",$F$2*E11,"")</f>
+        <v>3.0249323992110222</v>
+      </c>
+      <c r="H12" s="14">
+        <f t="shared" si="4"/>
+        <v>99.350879719686816</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="5"/>
+        <v>8.5621516744097598E-2</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="10"/>
+        <v>2.3506727552786097</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="6"/>
+        <v>31.926720873711989</v>
+      </c>
+      <c r="M12" s="8">
+        <v>8</v>
+      </c>
+      <c r="N12" s="15">
+        <v>1.877</v>
+      </c>
+      <c r="O12" s="9">
+        <f t="shared" si="3"/>
+        <v>2.9145962732919255</v>
+      </c>
+      <c r="P12" s="9">
+        <f t="shared" si="1"/>
+        <v>1.5749681725242082</v>
+      </c>
+      <c r="Q12" s="9">
+        <f t="shared" si="7"/>
+        <v>1.621205599577149</v>
+      </c>
+      <c r="R12" s="14">
+        <f t="shared" si="8"/>
+        <v>1.044056406127684</v>
+      </c>
+      <c r="S12" s="10">
+        <f t="shared" si="9"/>
+        <v>0.44376323594689182</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8">
+        <v>113892</v>
+      </c>
+      <c r="D13" s="14">
+        <v>323.47199999999998</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="2"/>
+        <v>2.9770832182892484</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.89991460251341027</v>
+      </c>
+      <c r="G13" s="9">
+        <f>IF(E12&lt;&gt;"",$F$2*E12,"")</f>
+        <v>2.8981519204717108</v>
+      </c>
+      <c r="H13" s="14">
+        <f t="shared" si="4"/>
+        <v>314.89579876693324</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="5"/>
+        <v>2.6512963202585511E-2</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="10"/>
+        <v>2.0593190902230316</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="6"/>
+        <v>65.74730578345725</v>
+      </c>
+      <c r="M13" s="8">
+        <v>9</v>
+      </c>
+      <c r="N13" s="15">
+        <v>5.2220000000000004</v>
+      </c>
+      <c r="O13" s="9">
+        <f t="shared" si="3"/>
+        <v>2.7820990942994142</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" si="1"/>
+        <v>0.95454012612084316</v>
+      </c>
+      <c r="Q13" s="9">
+        <f t="shared" si="7"/>
+        <v>2.5533472204520358</v>
+      </c>
+      <c r="R13" s="14">
+        <f t="shared" si="8"/>
+        <v>4.792632732788471</v>
+      </c>
+      <c r="S13" s="10">
+        <f t="shared" si="9"/>
+        <v>8.2222762775091801E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="8">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8">
+        <v>178495</v>
+      </c>
+      <c r="D14" s="14">
+        <v>770.24300000000005</v>
+      </c>
+      <c r="E14" s="9">
+        <f>IF(D13&lt;&gt;0,IF(D14&lt;&gt;0,D14/D13,""),"")</f>
+        <v>2.3811736409952022</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.79983442396464832</v>
+      </c>
+      <c r="G14" s="9">
+        <f>IF(E13&lt;&gt;"",$F$2*E13,"")</f>
+        <v>2.6080892335347765</v>
+      </c>
+      <c r="H14" s="14">
+        <f t="shared" si="4"/>
+        <v>843.64384054996117</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="5"/>
+        <v>9.5295693112382868E-2</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="10"/>
+        <v>1.8040771969786076</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="6"/>
+        <v>118.61321512671495</v>
+      </c>
+      <c r="M14" s="8">
+        <v>10</v>
+      </c>
+      <c r="N14" s="15">
+        <v>10.978999999999999</v>
+      </c>
+      <c r="O14" s="9">
+        <f>IF(N13&lt;&gt;0,IF(N14&lt;&gt;0,N14/N13,""),"")</f>
+        <v>2.1024511681348139</v>
+      </c>
+      <c r="P14" s="9">
+        <f t="shared" si="1"/>
+        <v>0.75570678716756901</v>
+      </c>
+      <c r="Q14" s="9">
+        <f t="shared" si="7"/>
+        <v>2.4372723778405905</v>
+      </c>
+      <c r="R14" s="14">
+        <f t="shared" si="8"/>
+        <v>12.727436357083565</v>
+      </c>
+      <c r="S14" s="10">
+        <f t="shared" si="9"/>
+        <v>0.15925278778427601</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8">
+        <v>179196</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1414.9190000000001</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" ref="E15:E19" si="11">IF(D14&lt;&gt;0,IF(D15&lt;&gt;0,D15/D14,""),"")</f>
+        <v>1.8369774214111652</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.77145882592728832</v>
+      </c>
+      <c r="G15" s="9">
+        <f>IF(E14&lt;&gt;"",$F$2*E14,"")</f>
+        <v>2.0860395497526887</v>
+      </c>
+      <c r="H15" s="14">
+        <f t="shared" si="4"/>
+        <v>1606.7573609201604</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="5"/>
+        <v>0.13558257463512774</v>
+      </c>
+      <c r="J15" s="9">
+        <f>J14*$F$2</f>
+        <v>1.580471209202307</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="6"/>
+        <v>187.46477153869253</v>
+      </c>
+      <c r="M15" s="8">
+        <v>11</v>
+      </c>
+      <c r="N15" s="14">
+        <v>15.02</v>
+      </c>
+      <c r="O15" s="9">
+        <f t="shared" ref="O15:O19" si="12">IF(N14&lt;&gt;0,IF(N15&lt;&gt;0,N15/N14,""),"")</f>
+        <v>1.3680663084069589</v>
+      </c>
+      <c r="P15" s="9">
+        <f t="shared" si="1"/>
+        <v>0.65070063416532842</v>
+      </c>
+      <c r="Q15" s="9">
+        <f t="shared" si="7"/>
+        <v>1.841863278110174</v>
+      </c>
+      <c r="R15" s="14">
+        <f t="shared" si="8"/>
+        <v>20.221816930371599</v>
+      </c>
+      <c r="S15" s="10">
+        <f t="shared" si="9"/>
+        <v>0.34632602732167772</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>12</v>
+      </c>
+      <c r="C16" s="8">
+        <v>89728</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2053.6469999999999</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" si="11"/>
+        <v>1.4514237210751992</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" ref="F16:F19" si="13">IF(E15&lt;&gt;0,IF(E16&lt;&gt;"",E16/E15,""),"")</f>
+        <v>0.79011516644565849</v>
+      </c>
+      <c r="G16" s="9">
+        <f>IF(E15&lt;&gt;"",$F$2*E15,"")</f>
+        <v>1.6092936218900986</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" si="4"/>
+        <v>2277.0201221911166</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="5"/>
+        <v>0.1087689959331456</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="10"/>
+        <v>1.3845800209108359</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="6"/>
+        <v>259.55997729708798</v>
+      </c>
+      <c r="M16" s="8">
+        <v>12</v>
+      </c>
+      <c r="N16" s="14">
+        <v>20.007000000000001</v>
+      </c>
+      <c r="O16" s="9">
+        <f t="shared" si="12"/>
+        <v>1.33202396804261</v>
+      </c>
+      <c r="P16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.9736545369600409</v>
+      </c>
+      <c r="Q16" s="9">
+        <f t="shared" si="7"/>
+        <v>1.198501603112121</v>
+      </c>
+      <c r="R16" s="14">
+        <f t="shared" si="8"/>
+        <v>18.001494078744056</v>
+      </c>
+      <c r="S16" s="10">
+        <f t="shared" si="9"/>
+        <v>0.10024021198860127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>13</v>
+      </c>
+      <c r="C17" s="8">
+        <v>16176</v>
+      </c>
+      <c r="D17" s="14">
+        <v>2282.8879999999999</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" si="11"/>
+        <v>1.1116262921524487</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="13"/>
+        <v>0.76588681582864571</v>
+      </c>
+      <c r="G17" s="9">
+        <f>IF(E16&lt;&gt;"",$F$2*E16,"")</f>
+        <v>1.2715272979196317</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" si="4"/>
+        <v>2611.2682207907578</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="5"/>
+        <v>0.14384420996157407</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" si="10"/>
+        <v>1.2129685268186741</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="6"/>
+        <v>314.83808328313728</v>
+      </c>
+      <c r="M17" s="8">
+        <v>13</v>
+      </c>
+      <c r="N17" s="14">
+        <v>19.690999999999999</v>
+      </c>
+      <c r="O17" s="9">
+        <f t="shared" si="12"/>
+        <v>0.98420552806517703</v>
+      </c>
+      <c r="P17" s="9">
+        <f t="shared" si="1"/>
+        <v>0.73887974366666453</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="7"/>
+        <v>1.1669265234239987</v>
+      </c>
+      <c r="R17" s="14">
+        <f t="shared" si="8"/>
+        <v>23.346698954143942</v>
+      </c>
+      <c r="S17" s="10">
+        <f t="shared" si="9"/>
+        <v>0.18565329105398121</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>14</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1488</v>
+      </c>
+      <c r="D18" s="14">
+        <v>2310.9540000000002</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="11"/>
+        <v>1.0122940766257478</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="13"/>
+        <v>0.91064243781571297</v>
+      </c>
+      <c r="G18" s="9">
+        <f>IF(E17&lt;&gt;"",$F$2*E17,"")</f>
+        <v>0.97384599344286848</v>
+      </c>
+      <c r="H18" s="14">
+        <f t="shared" si="4"/>
+        <v>2223.181332278803</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="5"/>
+        <v>3.7981140135717628E-2</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="10"/>
+        <v>1.0626273850786792</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="6"/>
+        <v>334.5555691623436</v>
+      </c>
+      <c r="M18" s="8">
+        <v>14</v>
+      </c>
+      <c r="N18" s="14">
+        <v>20.395</v>
+      </c>
+      <c r="O18" s="9">
+        <f t="shared" si="12"/>
+        <v>1.0357523741810979</v>
+      </c>
+      <c r="P18" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0523740668448138</v>
+      </c>
+      <c r="Q18" s="9">
+        <f t="shared" si="7"/>
+        <v>0.86221837050535621</v>
+      </c>
+      <c r="R18" s="14">
+        <f t="shared" si="8"/>
+        <v>16.977941933620968</v>
+      </c>
+      <c r="S18" s="10">
+        <f t="shared" si="9"/>
+        <v>0.16754391107521605</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>15</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="9" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="F19" s="9" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="G19" s="9">
+        <f>IF(E18&lt;&gt;"",$F$2*E18,"")</f>
+        <v>0.88682548952587859</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="4"/>
+        <v>2049.4129123217872</v>
+      </c>
+      <c r="I19" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" si="10"/>
+        <v>0.93092024611777202</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="6"/>
+        <v>311.44455278468018</v>
+      </c>
+      <c r="M19" s="8">
+        <v>15</v>
+      </c>
+      <c r="N19" s="14"/>
+      <c r="O19" s="9" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="P19" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q19" s="9">
+        <f t="shared" si="7"/>
+        <v>0.90737625307703018</v>
+      </c>
+      <c r="R19" s="14">
+        <f t="shared" si="8"/>
+        <v>18.505938681506031</v>
+      </c>
+      <c r="S19" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Thistlethwaite method implemented successfully
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Exponential Growth.xlsx
+++ b/Dissertation/Research/Exponential Growth.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="3" activeTab="3" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
   </bookViews>
   <sheets>
     <sheet name="G3 - None" sheetId="1" r:id="rId1"/>
@@ -9972,7 +9972,7 @@
   <dimension ref="B2:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10000,11 +10000,11 @@
       </c>
       <c r="E2" s="3">
         <f>AVERAGE(E6:E19)</f>
-        <v>3.1059535652336456</v>
+        <v>2.9579764028214695</v>
       </c>
       <c r="F2" s="3">
         <f>AVERAGE(F6:F19)</f>
-        <v>0.87605519977150292</v>
+        <v>0.88725959074094141</v>
       </c>
     </row>
     <row r="4" spans="2:19" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -10170,24 +10170,24 @@
         <v>0.96893491124260378</v>
       </c>
       <c r="G7" s="9">
-        <f>IF(E6&lt;&gt;"",$F$2*E6,"")</f>
-        <v>4.5554870388118145</v>
+        <f t="shared" ref="G7:G19" si="4">IF(E6&lt;&gt;"",$F$2*E6,"")</f>
+        <v>4.6137498718528951</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" ref="H7:H19" si="4">IF(D6&lt;&gt;0, D6*G7,"")</f>
-        <v>0.11844266300910718</v>
+        <f t="shared" ref="H7:H19" si="5">IF(D6&lt;&gt;0, D6*G7,"")</f>
+        <v>0.11995749666817526</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" ref="I7:I19" si="5">IF(D7&lt;&gt;0,((ABS(H7-D7))/D7),"")</f>
-        <v>9.5857534281624635E-2</v>
+        <f t="shared" ref="I7:I19" si="6">IF(D7&lt;&gt;0,((ABS(H7-D7))/D7),"")</f>
+        <v>8.4293918563547662E-2</v>
       </c>
       <c r="J7" s="9">
         <f>J6*$F$2</f>
-        <v>4.5554870388118145</v>
+        <v>4.6137498718528951</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" ref="K7:K19" si="6">J7*K6</f>
-        <v>0.11844266300910715</v>
+        <f t="shared" ref="K7:K19" si="7">J7*K6</f>
+        <v>0.11995749666817525</v>
       </c>
       <c r="M7" s="8">
         <v>3</v>
@@ -10204,16 +10204,16 @@
         <v>0.41331434674261303</v>
       </c>
       <c r="Q7" s="9">
-        <f t="shared" ref="Q7:Q19" si="7">IF(O6&lt;&gt;"",$F$2*O6,"")</f>
-        <v>1.0797889671602245</v>
+        <f t="shared" ref="Q7:Q19" si="8">IF(O6&lt;&gt;"",$F$2*O6,"")</f>
+        <v>1.0935990304481371</v>
       </c>
       <c r="R7" s="14">
-        <f t="shared" ref="R7:R19" si="8">IF(N6&lt;&gt;0, N6*Q7,"")</f>
-        <v>5.7228815259491903E-2</v>
+        <f t="shared" ref="R7:R19" si="9">IF(N6&lt;&gt;0, N6*Q7,"")</f>
+        <v>5.7960748613751265E-2</v>
       </c>
       <c r="S7" s="10">
-        <f t="shared" ref="S7:S19" si="9">IF(N7&lt;&gt;0,((ABS(R7-N7))/N7),"")</f>
-        <v>1.1195857503515521</v>
+        <f t="shared" ref="S7:S19" si="10">IF(N7&lt;&gt;0,((ABS(R7-N7))/N7),"")</f>
+        <v>1.1466943931018987</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
@@ -10235,24 +10235,24 @@
         <v>0.9378241361226034</v>
       </c>
       <c r="G8" s="9">
-        <f>IF(E7&lt;&gt;"",$F$2*E7,"")</f>
-        <v>4.413970429617958</v>
+        <f t="shared" si="4"/>
+        <v>4.470423322579359</v>
       </c>
       <c r="H8" s="14">
-        <f t="shared" si="4"/>
-        <v>0.57823012627995252</v>
+        <f t="shared" si="5"/>
+        <v>0.58562545525789611</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" si="5"/>
-        <v>6.5864093247249567E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.3916873573673481E-2</v>
       </c>
       <c r="J8" s="9">
-        <f t="shared" ref="J8:J19" si="10">J7*$F$2</f>
-        <v>3.9908581078427763</v>
+        <f t="shared" ref="J8:J19" si="11">J7*$F$2</f>
+        <v>4.093593823081271</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" si="6"/>
-        <v>0.47268786198438495</v>
+        <f t="shared" si="7"/>
+        <v>0.49105726739313432</v>
       </c>
       <c r="M8" s="8">
         <v>4</v>
@@ -10269,16 +10269,16 @@
         <v>2.617283950617284</v>
       </c>
       <c r="Q8" s="9">
-        <f t="shared" si="7"/>
-        <v>0.44629227158170903</v>
+        <f t="shared" si="8"/>
+        <v>0.45200016886802674</v>
       </c>
       <c r="R8" s="14">
-        <f t="shared" si="8"/>
-        <v>1.2049891332706144E-2</v>
+        <f t="shared" si="9"/>
+        <v>1.2204004559436722E-2</v>
       </c>
       <c r="S8" s="10">
-        <f t="shared" si="9"/>
-        <v>0.66528079631371817</v>
+        <f t="shared" si="10"/>
+        <v>0.66099987334897992</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
@@ -10300,24 +10300,24 @@
         <v>0.92003361511218518</v>
       </c>
       <c r="G9" s="9">
-        <f>IF(E8&lt;&gt;"",$F$2*E8,"")</f>
-        <v>4.1395280050271781</v>
+        <f t="shared" si="4"/>
+        <v>4.1924708906003261</v>
       </c>
       <c r="H9" s="14">
-        <f t="shared" si="4"/>
-        <v>2.5623678351118233</v>
+        <f t="shared" si="5"/>
+        <v>2.5951394812816018</v>
       </c>
       <c r="I9" s="10">
-        <f t="shared" si="5"/>
-        <v>4.7800878813889461E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.5622637948122655E-2</v>
       </c>
       <c r="J9" s="9">
-        <f t="shared" si="10"/>
-        <v>3.4962119969259255</v>
+        <f t="shared" si="11"/>
+        <v>3.6320803801267343</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="6"/>
-        <v>1.6526169738710728</v>
+        <f t="shared" si="7"/>
+        <v>1.7835594664172507</v>
       </c>
       <c r="M9" s="8">
         <v>5</v>
@@ -10334,16 +10334,16 @@
         <v>4.916666666666667</v>
       </c>
       <c r="Q9" s="9">
-        <f t="shared" si="7"/>
-        <v>1.1680735996953371</v>
+        <f t="shared" si="8"/>
+        <v>1.1830127876545884</v>
       </c>
       <c r="R9" s="14">
-        <f t="shared" si="8"/>
-        <v>4.2050649589032131E-2</v>
+        <f t="shared" si="9"/>
+        <v>4.2588460355565176E-2</v>
       </c>
       <c r="S9" s="10">
-        <f t="shared" si="9"/>
-        <v>0.82181928140240623</v>
+        <f t="shared" si="10"/>
+        <v>0.81954042222218138</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
@@ -10365,24 +10365,24 @@
         <v>0.81308340103357324</v>
       </c>
       <c r="G10" s="9">
-        <f>IF(E9&lt;&gt;"",$F$2*E9,"")</f>
-        <v>3.8085049153232866</v>
+        <f t="shared" si="4"/>
+        <v>3.8572141497316208</v>
       </c>
       <c r="H10" s="14">
-        <f t="shared" si="4"/>
-        <v>10.248686727134963</v>
+        <f t="shared" si="5"/>
+        <v>10.379763276927791</v>
       </c>
       <c r="I10" s="10">
-        <f t="shared" si="5"/>
-        <v>7.7448142045307256E-2</v>
+        <f t="shared" si="6"/>
+        <v>9.1228267128657586E-2</v>
       </c>
       <c r="J10" s="9">
-        <f t="shared" si="10"/>
-        <v>3.0628746994104668</v>
+        <f t="shared" si="11"/>
+        <v>3.2225981516094491</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="6"/>
-        <v>5.061758717085997</v>
+        <f t="shared" si="7"/>
+        <v>5.7476954397617677</v>
       </c>
       <c r="M10" s="8">
         <v>6</v>
@@ -10399,16 +10399,16 @@
         <v>0.22493536340132148</v>
       </c>
       <c r="Q10" s="9">
-        <f t="shared" si="7"/>
-        <v>5.7430285318354075</v>
+        <f t="shared" si="8"/>
+        <v>5.816479539301727</v>
       </c>
       <c r="R10" s="14">
-        <f t="shared" si="8"/>
-        <v>1.3553547335131562</v>
+        <f t="shared" si="9"/>
+        <v>1.3726891712752074</v>
       </c>
       <c r="S10" s="10">
-        <f t="shared" si="9"/>
-        <v>2.894697510095277</v>
+        <f t="shared" si="10"/>
+        <v>2.9445091128597913</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
@@ -10430,24 +10430,24 @@
         <v>0.9768458999335794</v>
       </c>
       <c r="G11" s="9">
-        <f>IF(E10&lt;&gt;"",$F$2*E10,"")</f>
-        <v>3.0966321294041386</v>
+        <f t="shared" si="4"/>
+        <v>3.1362367993786084</v>
       </c>
       <c r="H11" s="14">
-        <f t="shared" si="4"/>
-        <v>29.455164814892168</v>
+        <f t="shared" si="5"/>
+        <v>29.831884435689325</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="5"/>
-        <v>0.10317973404907542</v>
+        <f t="shared" si="6"/>
+        <v>9.1709766298583489E-2</v>
       </c>
       <c r="J11" s="9">
-        <f t="shared" si="10"/>
-        <v>2.6832473066671185</v>
+        <f t="shared" si="11"/>
+        <v>2.8592811171195138</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="6"/>
-        <v>13.58195044461981</v>
+        <f t="shared" si="7"/>
+        <v>16.434277037864764</v>
       </c>
       <c r="M11" s="8">
         <v>7</v>
@@ -10464,16 +10464,16 @@
         <v>1.2549874488043335</v>
       </c>
       <c r="Q11" s="9">
-        <f t="shared" si="7"/>
-        <v>1.2918102098325552</v>
+        <f t="shared" si="8"/>
+        <v>1.3083319388891848</v>
       </c>
       <c r="R11" s="14">
-        <f t="shared" si="8"/>
-        <v>0.44954995302172918</v>
+        <f t="shared" si="9"/>
+        <v>0.45529951473343627</v>
       </c>
       <c r="S11" s="10">
-        <f t="shared" si="9"/>
-        <v>0.30194106673644538</v>
+        <f t="shared" si="10"/>
+        <v>0.29301317587975734</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
@@ -10495,24 +10495,24 @@
         <v>0.95808816131812446</v>
       </c>
       <c r="G12" s="9">
-        <f>IF(E11&lt;&gt;"",$F$2*E11,"")</f>
-        <v>3.0249323992110222</v>
+        <f t="shared" si="4"/>
+        <v>3.0636200586938056</v>
       </c>
       <c r="H12" s="14">
-        <f t="shared" si="4"/>
-        <v>99.350879719686816</v>
+        <f t="shared" si="5"/>
+        <v>100.62153720773935</v>
       </c>
       <c r="I12" s="10">
-        <f t="shared" si="5"/>
-        <v>8.5621516744097598E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.3926986510028589E-2</v>
       </c>
       <c r="J12" s="9">
-        <f t="shared" si="10"/>
-        <v>2.3506727552786097</v>
+        <f t="shared" si="11"/>
+        <v>2.5369245937887617</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="6"/>
-        <v>31.926720873711989</v>
+        <f t="shared" si="7"/>
+        <v>41.692521598497038</v>
       </c>
       <c r="M12" s="8">
         <v>8</v>
@@ -10529,16 +10529,16 @@
         <v>1.5749681725242082</v>
       </c>
       <c r="Q12" s="9">
-        <f t="shared" si="7"/>
-        <v>1.621205599577149</v>
+        <f t="shared" si="8"/>
+        <v>1.6419401621757652</v>
       </c>
       <c r="R12" s="14">
-        <f t="shared" si="8"/>
-        <v>1.044056406127684</v>
+        <f t="shared" si="9"/>
+        <v>1.0574094644411929</v>
       </c>
       <c r="S12" s="10">
-        <f t="shared" si="9"/>
-        <v>0.44376323594689182</v>
+        <f t="shared" si="10"/>
+        <v>0.43664919315866124</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
@@ -10560,24 +10560,24 @@
         <v>0.89991460251341027</v>
       </c>
       <c r="G13" s="9">
-        <f>IF(E12&lt;&gt;"",$F$2*E12,"")</f>
-        <v>2.8981519204717108</v>
+        <f t="shared" si="4"/>
+        <v>2.9352181090112728</v>
       </c>
       <c r="H13" s="14">
-        <f t="shared" si="4"/>
-        <v>314.89579876693324</v>
+        <f t="shared" si="5"/>
+        <v>318.92318841651081</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="5"/>
-        <v>2.6512963202585511E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.4062458523424498E-2</v>
       </c>
       <c r="J13" s="9">
-        <f t="shared" si="10"/>
-        <v>2.0593190902230316</v>
+        <f t="shared" si="11"/>
+        <v>2.2509106768256455</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="6"/>
-        <v>65.74730578345725</v>
+        <f t="shared" si="7"/>
+        <v>93.846142009840804</v>
       </c>
       <c r="M13" s="8">
         <v>9</v>
@@ -10594,16 +10594,16 @@
         <v>0.95454012612084316</v>
       </c>
       <c r="Q13" s="9">
-        <f t="shared" si="7"/>
-        <v>2.5533472204520358</v>
+        <f t="shared" si="8"/>
+        <v>2.5860034966160668</v>
       </c>
       <c r="R13" s="14">
-        <f t="shared" si="8"/>
-        <v>4.792632732788471</v>
+        <f t="shared" si="9"/>
+        <v>4.8539285631483571</v>
       </c>
       <c r="S13" s="10">
-        <f t="shared" si="9"/>
-        <v>8.2222762775091801E-2</v>
+        <f t="shared" si="10"/>
+        <v>7.0484763855159574E-2</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
@@ -10625,24 +10625,24 @@
         <v>0.79983442396464832</v>
       </c>
       <c r="G14" s="9">
-        <f>IF(E13&lt;&gt;"",$F$2*E13,"")</f>
-        <v>2.6080892335347765</v>
+        <f t="shared" si="4"/>
+        <v>2.6414456378610431</v>
       </c>
       <c r="H14" s="14">
-        <f t="shared" si="4"/>
-        <v>843.64384054996117</v>
+        <f t="shared" si="5"/>
+        <v>854.43370337018735</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="5"/>
-        <v>9.5295693112382868E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.1093040811408702</v>
       </c>
       <c r="J14" s="9">
-        <f t="shared" si="10"/>
-        <v>1.8040771969786076</v>
+        <f t="shared" si="11"/>
+        <v>1.9971420859147377</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="6"/>
-        <v>118.61321512671495</v>
+        <f t="shared" si="7"/>
+        <v>187.42407980858417</v>
       </c>
       <c r="M14" s="8">
         <v>10</v>
@@ -10659,16 +10659,16 @@
         <v>0.75570678716756901</v>
       </c>
       <c r="Q14" s="9">
-        <f t="shared" si="7"/>
-        <v>2.4372723778405905</v>
+        <f t="shared" si="8"/>
+        <v>2.4684441038088418</v>
       </c>
       <c r="R14" s="14">
-        <f t="shared" si="8"/>
-        <v>12.727436357083565</v>
+        <f t="shared" si="9"/>
+        <v>12.890215110089773</v>
       </c>
       <c r="S14" s="10">
-        <f t="shared" si="9"/>
-        <v>0.15925278778427601</v>
+        <f t="shared" si="10"/>
+        <v>0.17407916113396249</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
@@ -10682,7 +10682,7 @@
         <v>1414.9190000000001</v>
       </c>
       <c r="E15" s="9">
-        <f t="shared" ref="E15:E19" si="11">IF(D14&lt;&gt;0,IF(D15&lt;&gt;0,D15/D14,""),"")</f>
+        <f t="shared" ref="E15:E19" si="12">IF(D14&lt;&gt;0,IF(D15&lt;&gt;0,D15/D14,""),"")</f>
         <v>1.8369774214111652</v>
       </c>
       <c r="F15" s="9">
@@ -10690,24 +10690,24 @@
         <v>0.77145882592728832</v>
       </c>
       <c r="G15" s="9">
-        <f>IF(E14&lt;&gt;"",$F$2*E14,"")</f>
-        <v>2.0860395497526887</v>
+        <f t="shared" si="4"/>
+        <v>2.1127191501925204</v>
       </c>
       <c r="H15" s="14">
-        <f t="shared" si="4"/>
-        <v>1606.7573609201604</v>
+        <f t="shared" si="5"/>
+        <v>1627.3071364017376</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="5"/>
-        <v>0.13558257463512774</v>
+        <f t="shared" si="6"/>
+        <v>0.15010621555137607</v>
       </c>
       <c r="J15" s="9">
         <f>J14*$F$2</f>
-        <v>1.580471209202307</v>
+        <v>1.7719834698002201</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" si="6"/>
-        <v>187.46477153869253</v>
+        <f t="shared" si="7"/>
+        <v>332.11237126332833</v>
       </c>
       <c r="M15" s="8">
         <v>11</v>
@@ -10716,7 +10716,7 @@
         <v>15.02</v>
       </c>
       <c r="O15" s="9">
-        <f t="shared" ref="O15:O19" si="12">IF(N14&lt;&gt;0,IF(N15&lt;&gt;0,N15/N14,""),"")</f>
+        <f t="shared" ref="O15:O19" si="13">IF(N14&lt;&gt;0,IF(N15&lt;&gt;0,N15/N14,""),"")</f>
         <v>1.3680663084069589</v>
       </c>
       <c r="P15" s="9">
@@ -10724,16 +10724,16 @@
         <v>0.65070063416532842</v>
       </c>
       <c r="Q15" s="9">
-        <f t="shared" si="7"/>
-        <v>1.841863278110174</v>
+        <f t="shared" si="8"/>
+        <v>1.8654199629921091</v>
       </c>
       <c r="R15" s="14">
-        <f t="shared" si="8"/>
-        <v>20.221816930371599</v>
+        <f t="shared" si="9"/>
+        <v>20.480445773690363</v>
       </c>
       <c r="S15" s="10">
-        <f t="shared" si="9"/>
-        <v>0.34632602732167772</v>
+        <f t="shared" si="10"/>
+        <v>0.36354499159057013</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
@@ -10747,32 +10747,32 @@
         <v>2053.6469999999999</v>
       </c>
       <c r="E16" s="9">
+        <f t="shared" si="12"/>
+        <v>1.4514237210751992</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" ref="F16:F19" si="14">IF(E15&lt;&gt;0,IF(E16&lt;&gt;"",E16/E15,""),"")</f>
+        <v>0.79011516644565849</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="4"/>
+        <v>1.6298758351216203</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" si="5"/>
+        <v>2306.1422867544479</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="6"/>
+        <v>0.12294970204443509</v>
+      </c>
+      <c r="J16" s="9">
         <f t="shared" si="11"/>
-        <v>1.4514237210751992</v>
-      </c>
-      <c r="F16" s="9">
-        <f t="shared" ref="F16:F19" si="13">IF(E15&lt;&gt;0,IF(E16&lt;&gt;"",E16/E15,""),"")</f>
-        <v>0.79011516644565849</v>
-      </c>
-      <c r="G16" s="9">
-        <f>IF(E15&lt;&gt;"",$F$2*E15,"")</f>
-        <v>1.6092936218900986</v>
-      </c>
-      <c r="H16" s="14">
-        <f t="shared" si="4"/>
-        <v>2277.0201221911166</v>
-      </c>
-      <c r="I16" s="10">
-        <f t="shared" si="5"/>
-        <v>0.1087689959331456</v>
-      </c>
-      <c r="J16" s="9">
-        <f t="shared" si="10"/>
-        <v>1.3845800209108359</v>
+        <v>1.5722093282146565</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" si="6"/>
-        <v>259.55997729708798</v>
+        <f t="shared" si="7"/>
+        <v>522.15016811569399</v>
       </c>
       <c r="M16" s="8">
         <v>12</v>
@@ -10781,7 +10781,7 @@
         <v>20.007000000000001</v>
       </c>
       <c r="O16" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.33202396804261</v>
       </c>
       <c r="P16" s="9">
@@ -10789,16 +10789,16 @@
         <v>0.9736545369600409</v>
       </c>
       <c r="Q16" s="9">
-        <f t="shared" si="7"/>
-        <v>1.198501603112121</v>
+        <f t="shared" si="8"/>
+        <v>1.2138299529036289</v>
       </c>
       <c r="R16" s="14">
-        <f t="shared" si="8"/>
-        <v>18.001494078744056</v>
+        <f t="shared" si="9"/>
+        <v>18.231725892612506</v>
       </c>
       <c r="S16" s="10">
-        <f t="shared" si="9"/>
-        <v>0.10024021198860127</v>
+        <f t="shared" si="10"/>
+        <v>8.8732648942245002E-2</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
@@ -10812,32 +10812,32 @@
         <v>2282.8879999999999</v>
       </c>
       <c r="E17" s="9">
+        <f t="shared" si="12"/>
+        <v>1.1116262921524487</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="14"/>
+        <v>0.76588681582864571</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="4"/>
+        <v>1.2877896167528755</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" si="5"/>
+        <v>2644.6652830756925</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="6"/>
+        <v>0.15847351384548547</v>
+      </c>
+      <c r="J17" s="9">
         <f t="shared" si="11"/>
-        <v>1.1116262921524487</v>
-      </c>
-      <c r="F17" s="9">
-        <f t="shared" si="13"/>
-        <v>0.76588681582864571</v>
-      </c>
-      <c r="G17" s="9">
-        <f>IF(E16&lt;&gt;"",$F$2*E16,"")</f>
-        <v>1.2715272979196317</v>
-      </c>
-      <c r="H17" s="14">
-        <f t="shared" si="4"/>
-        <v>2611.2682207907578</v>
-      </c>
-      <c r="I17" s="10">
-        <f t="shared" si="5"/>
-        <v>0.14384420996157407</v>
-      </c>
-      <c r="J17" s="9">
-        <f t="shared" si="10"/>
-        <v>1.2129685268186741</v>
+        <v>1.3949578051108267</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" si="6"/>
-        <v>314.83808328313728</v>
+        <f t="shared" si="7"/>
+        <v>728.37745245291762</v>
       </c>
       <c r="M17" s="8">
         <v>13</v>
@@ -10846,7 +10846,7 @@
         <v>19.690999999999999</v>
       </c>
       <c r="O17" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.98420552806517703</v>
       </c>
       <c r="P17" s="9">
@@ -10854,16 +10854,16 @@
         <v>0.73887974366666453</v>
       </c>
       <c r="Q17" s="9">
-        <f t="shared" si="7"/>
-        <v>1.1669265234239987</v>
+        <f t="shared" si="8"/>
+        <v>1.181851040742611</v>
       </c>
       <c r="R17" s="14">
-        <f t="shared" si="8"/>
-        <v>23.346698954143942</v>
+        <f t="shared" si="9"/>
+        <v>23.645293772137421</v>
       </c>
       <c r="S17" s="10">
-        <f t="shared" si="9"/>
-        <v>0.18565329105398121</v>
+        <f t="shared" si="10"/>
+        <v>0.2008173161412535</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -10877,32 +10877,32 @@
         <v>2310.9540000000002</v>
       </c>
       <c r="E18" s="9">
+        <f t="shared" si="12"/>
+        <v>1.0122940766257478</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="14"/>
+        <v>0.91064243781571297</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="4"/>
+        <v>0.98630108903205183</v>
+      </c>
+      <c r="H18" s="14">
+        <f t="shared" si="5"/>
+        <v>2251.6149205382026</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="6"/>
+        <v>2.5677308791865871E-2</v>
+      </c>
+      <c r="J18" s="9">
         <f t="shared" si="11"/>
-        <v>1.0122940766257478</v>
-      </c>
-      <c r="F18" s="9">
-        <f t="shared" si="13"/>
-        <v>0.91064243781571297</v>
-      </c>
-      <c r="G18" s="9">
-        <f>IF(E17&lt;&gt;"",$F$2*E17,"")</f>
-        <v>0.97384599344286848</v>
-      </c>
-      <c r="H18" s="14">
-        <f t="shared" si="4"/>
-        <v>2223.181332278803</v>
-      </c>
-      <c r="I18" s="10">
-        <f t="shared" si="5"/>
-        <v>3.7981140135717628E-2</v>
-      </c>
-      <c r="J18" s="9">
-        <f t="shared" si="10"/>
-        <v>1.0626273850786792</v>
+        <v>1.237689691263514</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="6"/>
-        <v>334.5555691623436</v>
+        <f t="shared" si="7"/>
+        <v>901.50526424975646</v>
       </c>
       <c r="M18" s="8">
         <v>14</v>
@@ -10911,7 +10911,7 @@
         <v>20.395</v>
       </c>
       <c r="O18" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0357523741810979</v>
       </c>
       <c r="P18" s="9">
@@ -10919,75 +10919,81 @@
         <v>1.0523740668448138</v>
       </c>
       <c r="Q18" s="9">
-        <f t="shared" si="7"/>
-        <v>0.86221837050535621</v>
+        <f t="shared" si="8"/>
+        <v>0.87324579403608105</v>
       </c>
       <c r="R18" s="14">
-        <f t="shared" si="8"/>
-        <v>16.977941933620968</v>
+        <f t="shared" si="9"/>
+        <v>17.195082930364471</v>
       </c>
       <c r="S18" s="10">
-        <f t="shared" si="9"/>
-        <v>0.16754391107521605</v>
+        <f t="shared" si="10"/>
+        <v>0.15689713506425734</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>15</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="9" t="str">
+      <c r="C19" s="8">
+        <v>144</v>
+      </c>
+      <c r="D19" s="14">
+        <v>2390.1579999999999</v>
+      </c>
+      <c r="E19" s="9">
+        <f t="shared" si="12"/>
+        <v>1.0342732914631791</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="14"/>
+        <v>1.0217122823742031</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="4"/>
+        <v>0.89816762813644013</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="5"/>
+        <v>2075.6240729124193</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="6"/>
+        <v>0.13159545397734404</v>
+      </c>
+      <c r="J19" s="9">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="F19" s="9" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G19" s="9">
-        <f>IF(E18&lt;&gt;"",$F$2*E18,"")</f>
-        <v>0.88682548952587859</v>
-      </c>
-      <c r="H19" s="14">
-        <f t="shared" si="4"/>
-        <v>2049.4129123217872</v>
-      </c>
-      <c r="I19" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="J19" s="9">
-        <f t="shared" si="10"/>
-        <v>0.93092024611777202</v>
+        <v>1.0981520489347476</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="6"/>
-        <v>311.44455278468018</v>
+        <f t="shared" si="7"/>
+        <v>989.98985306133113</v>
       </c>
       <c r="M19" s="8">
         <v>15</v>
       </c>
-      <c r="N19" s="14"/>
-      <c r="O19" s="9" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="P19" s="9" t="str">
+      <c r="N19" s="14">
+        <v>20.925999999999998</v>
+      </c>
+      <c r="O19" s="9">
+        <f t="shared" si="13"/>
+        <v>1.0260357930865407</v>
+      </c>
+      <c r="P19" s="9">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.99061881841956723</v>
       </c>
       <c r="Q19" s="9">
-        <f t="shared" si="7"/>
-        <v>0.90737625307703018</v>
+        <f t="shared" si="8"/>
+        <v>0.91898122762487933</v>
       </c>
       <c r="R19" s="14">
-        <f t="shared" si="8"/>
-        <v>18.505938681506031</v>
-      </c>
-      <c r="S19" s="10" t="str">
         <f t="shared" si="9"/>
-        <v/>
+        <v>18.742622137409413</v>
+      </c>
+      <c r="S19" s="10">
+        <f t="shared" si="10"/>
+        <v>0.10433804179444643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition to previous commit, some files blocked
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Exponential Growth.xlsx
+++ b/Dissertation/Research/Exponential Growth.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="4" xr2:uid="{A8CCEC81-E18C-41F8-B666-97099CC371C2}"/>
   </bookViews>
   <sheets>
     <sheet name="G3 - None" sheetId="1" r:id="rId1"/>
     <sheet name="G3 - Dup Check" sheetId="2" r:id="rId2"/>
     <sheet name="G0 - Dup Check" sheetId="4" r:id="rId3"/>
     <sheet name="Phase 4 Generation" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171026"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="26">
   <si>
     <t>Depth</t>
   </si>
@@ -72,6 +73,39 @@
   </si>
   <si>
     <t>Pos Count</t>
+  </si>
+  <si>
+    <t>Quarter Turns</t>
+  </si>
+  <si>
+    <t>Half Turns</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>OBROWROGRWWWBRBWWWGOGWOYGGGWRYBBBYYYBOBYYYGRGOGROYROBR</t>
+  </si>
+  <si>
+    <t>WBWWWWWGWOOOGWGRRRBWBBOGOGRGRBRBOOOOGYGRRRBYBYGYYYYYBY</t>
+  </si>
+  <si>
+    <t>YWRBWYOOWOOBYYOGBYBRGGOGWGWBRYGBOWRRGWBRRYGRBWOWYYBOGR</t>
+  </si>
+  <si>
+    <t>OGOYWYRBRWOWGOBWRWBRGGOBWGYBRGWBYYOYBRGYRYGOBOBOWYWRGR</t>
+  </si>
+  <si>
+    <t>GYWBWRBOYWRWRWRGWBOGRBORYGRGRBOBWWGBYYOYOOGYORBBWYGGOY</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
   </si>
 </sst>
 </file>
@@ -119,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -170,6 +204,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9971,7 +10011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C26503-4535-4175-8A49-8C86F5FB11B3}">
   <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -11000,4 +11040,224 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5E71B9-550C-40AC-A023-4F20D495B8D7}">
+  <dimension ref="B3:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="73.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
+      <c r="C5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>192</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>237</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1227</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3">
+        <v>286252</v>
+      </c>
+      <c r="G8" s="3">
+        <v>180.63300000000001</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>246</v>
+      </c>
+      <c r="J8" s="3">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3">
+        <v>507904</v>
+      </c>
+      <c r="L8" s="3">
+        <v>418.13299999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
+        <v>237</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>30537</v>
+      </c>
+      <c r="E10" s="3">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3">
+        <v>21814238</v>
+      </c>
+      <c r="G10" s="3">
+        <v>13324.681</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added phase one monochrome conversion, initial tests show great optimisation with same output
</commit_message>
<xml_diff>
--- a/Dissertation/Research/Exponential Growth.xlsx
+++ b/Dissertation/Research/Exponential Growth.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="27">
   <si>
     <t>Depth</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -11044,10 +11047,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5E71B9-550C-40AC-A023-4F20D495B8D7}">
-  <dimension ref="B3:L10"/>
+  <dimension ref="B3:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11057,7 +11060,7 @@
     <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>17</v>
       </c>
@@ -11068,15 +11071,17 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="18"/>
       <c r="C4" s="18" t="s">
         <v>24</v>
@@ -11087,21 +11092,23 @@
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="18"/>
+      <c r="K4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
       <c r="C5" s="17" t="s">
         <v>0</v>
@@ -11115,22 +11122,32 @@
       <c r="F5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H5" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="K5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="L5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="18"/>
+      <c r="M5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -11147,10 +11164,33 @@
         <v>21</v>
       </c>
       <c r="G6" s="3">
+        <f>F6+D6</f>
+        <v>213</v>
+      </c>
+      <c r="H6" s="3">
         <v>0.15</v>
       </c>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>480</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>23</v>
+      </c>
+      <c r="M6" s="3">
+        <f>L6+J6</f>
+        <v>503</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.503</v>
+      </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
@@ -11167,10 +11207,33 @@
         <v>237</v>
       </c>
       <c r="G7" s="3">
+        <f t="shared" ref="G7:G10" si="0">F7+D7</f>
+        <v>267</v>
+      </c>
+      <c r="H7" s="3">
         <v>0.218</v>
       </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>50</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>180</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" ref="M7:M10" si="1">L7+J7</f>
+        <v>230</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.316</v>
+      </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -11187,25 +11250,33 @@
         <v>286252</v>
       </c>
       <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>287479</v>
+      </c>
+      <c r="H8" s="3">
         <v>180.63300000000001</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>2</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>246</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>6</v>
       </c>
-      <c r="K8" s="3">
-        <v>507904</v>
-      </c>
       <c r="L8" s="3">
-        <v>418.13299999999998</v>
+        <v>451204</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="1"/>
+        <v>451450</v>
+      </c>
+      <c r="N8" s="3">
+        <v>429.428</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
@@ -11222,10 +11293,33 @@
         <v>237</v>
       </c>
       <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>237</v>
+      </c>
+      <c r="H9" s="3">
         <v>0.187</v>
       </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>3</v>
+      </c>
+      <c r="L9" s="3">
+        <v>180</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.22800000000000001</v>
+      </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -11242,20 +11336,28 @@
         <v>21814238</v>
       </c>
       <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>21844775</v>
+      </c>
+      <c r="H10" s="3">
         <v>13324.681</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>